<commit_message>
📝 Update journal de travail
</commit_message>
<xml_diff>
--- a/Journal de travail/Journal-de-Travail_NomPrénom.xlsx
+++ b/Journal de travail/Journal-de-Travail_NomPrénom.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pt52png\Documents\GitHub\P_mobile\Journal de travail\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51AA1EED-976B-446F-A834-45705CF70826}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79AA55E9-C492-4AD6-95F8-060609CA7B73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -134,6 +134,9 @@
   </si>
   <si>
     <t xml:space="preserve">Création du github et création des dossiers du projet </t>
+  </si>
+  <si>
+    <t>prise de mesure de l'écran du téléphone pour la maquette et commencement de la page d'accueil</t>
   </si>
 </sst>
 </file>
@@ -433,13 +436,6 @@
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="20" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -457,85 +453,18 @@
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="20" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="17">
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCCC00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -705,6 +634,80 @@
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="2" tint="-9.9978637043366805E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCCC00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="-0.24994659260841701"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1083,7 +1086,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>3.125E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>6.9444444444444441E-3</c:v>
@@ -1792,18 +1795,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F2213DF1-F6B1-174C-AC17-4E96BE96C00D}" name="Table1" displayName="Table1" ref="A6:G532" totalsRowShown="0" headerRowDxfId="16" tableBorderDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F2213DF1-F6B1-174C-AC17-4E96BE96C00D}" name="Table1" displayName="Table1" ref="A6:G532" totalsRowShown="0" headerRowDxfId="8" tableBorderDxfId="7">
   <autoFilter ref="A6:G532" xr:uid="{F2213DF1-F6B1-174C-AC17-4E96BE96C00D}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{315BA4B4-9BD9-AB4E-8D40-FABFA0BB2AEA}" name="Semaine" dataDxfId="14">
+    <tableColumn id="1" xr3:uid="{315BA4B4-9BD9-AB4E-8D40-FABFA0BB2AEA}" name="Semaine" dataDxfId="6">
       <calculatedColumnFormula>IF(ISBLANK(#REF!),"",_xlfn.ISOWEEKNUM('Journal de travail'!#REF!))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{503C31E9-854D-BF42-85AC-8DFA1376C4D8}" name="Jour" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{B35A0B98-71A0-BA4F-BFAB-00A05EA1F23A}" name="heure" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{BE4D837D-FC99-BA48-A82F-B8C8E4CE5BF8}" name="min." dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{A2DCC539-6D2A-B04A-BF8E-6FACE6268D1F}" name="Activité" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{4EA406B9-7EF7-D547-AF98-5AD11BE168E9}" name="Description" dataDxfId="9"/>
-    <tableColumn id="7" xr3:uid="{1735360B-2647-6D42-A0E3-3425EE302FFD}" name="Remarque / problème" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{503C31E9-854D-BF42-85AC-8DFA1376C4D8}" name="Jour" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{B35A0B98-71A0-BA4F-BFAB-00A05EA1F23A}" name="heure" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{BE4D837D-FC99-BA48-A82F-B8C8E4CE5BF8}" name="min." dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{A2DCC539-6D2A-B04A-BF8E-6FACE6268D1F}" name="Activité" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{4EA406B9-7EF7-D547-AF98-5AD11BE168E9}" name="Description" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{1735360B-2647-6D42-A0E3-3425EE302FFD}" name="Remarque / problème" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1999,7 +2002,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
+      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2034,11 +2037,11 @@
       <c r="B2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="53" t="s">
+      <c r="C2" s="58" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
       <c r="F2" s="5" t="s">
         <v>2</v>
       </c>
@@ -2052,7 +2055,7 @@
       </c>
       <c r="C3" s="22" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 1 heurs 30 minutes</v>
+        <v>0 jours 2 heurs 15 minutes</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="3"/>
@@ -2071,20 +2074,20 @@
       </c>
       <c r="D4" s="22">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>30</v>
+        <v>75</v>
       </c>
       <c r="E4" s="40">
         <f>SUM(C4:D4)</f>
-        <v>90</v>
+        <v>135</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C5" s="54" t="s">
+      <c r="C5" s="59" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="54"/>
+      <c r="D5" s="59"/>
     </row>
     <row r="6" spans="1:15" s="20" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="18" t="s">
@@ -2126,19 +2129,19 @@
         <f>IF(ISBLANK(B7),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B7))</f>
         <v/>
       </c>
-      <c r="B8" s="55">
+      <c r="B8" s="53">
         <v>45737</v>
       </c>
-      <c r="C8" s="56">
+      <c r="C8" s="54">
         <v>1</v>
       </c>
-      <c r="D8" s="57">
+      <c r="D8" s="55">
         <v>20</v>
       </c>
-      <c r="E8" s="58" t="s">
+      <c r="E8" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="59" t="s">
+      <c r="F8" s="57" t="s">
         <v>29</v>
       </c>
       <c r="G8" s="51"/>
@@ -2182,15 +2185,23 @@
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="str">
+      <c r="A10" s="8">
         <f>IF(ISBLANK(B10),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B10))</f>
-        <v/>
-      </c>
-      <c r="B10" s="42"/>
+        <v>12</v>
+      </c>
+      <c r="B10" s="42">
+        <v>45737</v>
+      </c>
       <c r="C10" s="43"/>
-      <c r="D10" s="44"/>
-      <c r="E10" s="45"/>
-      <c r="F10" s="36"/>
+      <c r="D10" s="44">
+        <v>45</v>
+      </c>
+      <c r="E10" s="45" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" s="36" t="s">
+        <v>31</v>
+      </c>
       <c r="G10" s="51"/>
       <c r="M10" t="s">
         <v>5</v>
@@ -8530,28 +8541,28 @@
     <mergeCell ref="C5:D5"/>
   </mergeCells>
   <conditionalFormatting sqref="E9:E532 E7">
-    <cfRule type="expression" dxfId="7" priority="1">
+    <cfRule type="expression" dxfId="16" priority="1">
       <formula>$E7="Autre"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="2" stopIfTrue="1">
       <formula>$E7="Design"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="3" stopIfTrue="1">
       <formula>$E7="Présentation"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="4" stopIfTrue="1">
       <formula>$E7="Meeting"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="5" stopIfTrue="1">
       <formula>$E7="Documentation"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="6" stopIfTrue="1">
       <formula>$E7="Test"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="7" stopIfTrue="1">
       <formula>$E7="Analyse"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="9" stopIfTrue="1">
       <formula>$E7="Développement"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8719,7 +8730,7 @@
       </c>
       <c r="B10">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C10,'Journal de travail'!$D$7:$D$532)</f>
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="C10" s="37" t="str">
         <f>'Journal de travail'!M14</f>
@@ -8727,7 +8738,7 @@
       </c>
       <c r="D10" s="33">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3.125E-2</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -8754,7 +8765,7 @@
       </c>
       <c r="D12" s="34">
         <f>SUM(D4:D11)</f>
-        <v>6.25E-2</v>
+        <v>9.375E-2</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -8991,6 +9002,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
@@ -8999,15 +9019,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9030,6 +9041,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -9038,12 +9057,4 @@
     <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
mis a jour du journal de travail pour la semaine 2
</commit_message>
<xml_diff>
--- a/Journal de travail/Journal-de-Travail_NomPrénom.xlsx
+++ b/Journal de travail/Journal-de-Travail_NomPrénom.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pt52png\Documents\GitHub\P_mobile\Journal de travail\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79AA55E9-C492-4AD6-95F8-060609CA7B73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5044DD09-35FD-42EB-8EC6-BFD28C5BB7E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -137,6 +137,15 @@
   </si>
   <si>
     <t>prise de mesure de l'écran du téléphone pour la maquette et commencement de la page d'accueil</t>
+  </si>
+  <si>
+    <t>introduction de Monsieur Benfares</t>
+  </si>
+  <si>
+    <t xml:space="preserve">finalisation de la maquette </t>
+  </si>
+  <si>
+    <t>commencement du developpement de l'application (page d'accueil)</t>
   </si>
 </sst>
 </file>
@@ -1071,7 +1080,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>4.5138888888888888E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1080,13 +1089,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.5555555555555552E-2</c:v>
+                  <c:v>7.6388888888888895E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.125E-2</c:v>
+                  <c:v>5.9027777777777776E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>6.9444444444444441E-3</c:v>
@@ -2002,7 +2011,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
+      <selection pane="bottomLeft" activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2055,7 +2064,7 @@
       </c>
       <c r="C3" s="22" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 2 heurs 15 minutes</v>
+        <v>0 jours 4 heurs 30 minutes</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="3"/>
@@ -2070,15 +2079,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="22">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="D4" s="22">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>75</v>
+        <v>150</v>
       </c>
       <c r="E4" s="40">
         <f>SUM(C4:D4)</f>
-        <v>135</v>
+        <v>270</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2214,15 +2223,23 @@
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="16" t="str">
+      <c r="A11" s="16">
         <f>IF(ISBLANK(B11),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B11))</f>
-        <v/>
-      </c>
-      <c r="B11" s="46"/>
+        <v>13</v>
+      </c>
+      <c r="B11" s="46">
+        <v>45744</v>
+      </c>
       <c r="C11" s="47"/>
-      <c r="D11" s="48"/>
-      <c r="E11" s="49"/>
-      <c r="F11" s="36"/>
+      <c r="D11" s="48">
+        <v>30</v>
+      </c>
+      <c r="E11" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="36" t="s">
+        <v>32</v>
+      </c>
       <c r="G11" s="52"/>
       <c r="M11" t="s">
         <v>6</v>
@@ -2235,15 +2252,23 @@
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="str">
+      <c r="A12" s="8">
         <f>IF(ISBLANK(B12),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B12))</f>
-        <v/>
-      </c>
-      <c r="B12" s="42"/>
+        <v>13</v>
+      </c>
+      <c r="B12" s="42">
+        <v>45744</v>
+      </c>
       <c r="C12" s="43"/>
-      <c r="D12" s="44"/>
-      <c r="E12" s="45"/>
-      <c r="F12" s="36"/>
+      <c r="D12" s="44">
+        <v>40</v>
+      </c>
+      <c r="E12" s="45" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" s="36" t="s">
+        <v>33</v>
+      </c>
       <c r="G12" s="51"/>
       <c r="M12" t="s">
         <v>7</v>
@@ -2256,15 +2281,25 @@
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="16" t="str">
+      <c r="A13" s="16">
         <f>IF(ISBLANK(B13),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B13))</f>
-        <v/>
-      </c>
-      <c r="B13" s="46"/>
-      <c r="C13" s="47"/>
-      <c r="D13" s="48"/>
-      <c r="E13" s="49"/>
-      <c r="F13" s="36"/>
+        <v>13</v>
+      </c>
+      <c r="B13" s="46">
+        <v>45744</v>
+      </c>
+      <c r="C13" s="47">
+        <v>1</v>
+      </c>
+      <c r="D13" s="48">
+        <v>5</v>
+      </c>
+      <c r="E13" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="F13" s="36" t="s">
+        <v>34</v>
+      </c>
       <c r="G13" s="52"/>
       <c r="M13" t="s">
         <v>8</v>
@@ -8636,11 +8671,11 @@
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C5" s="41" t="str">
         <f>'Journal de travail'!M9</f>
@@ -8648,7 +8683,7 @@
       </c>
       <c r="D5" s="33">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>0</v>
+        <v>4.5138888888888888E-2</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -8694,7 +8729,7 @@
       </c>
       <c r="B8">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C8,'Journal de travail'!$D$7:$D$532)</f>
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="C8" s="28" t="str">
         <f>'Journal de travail'!M12</f>
@@ -8702,7 +8737,7 @@
       </c>
       <c r="D8" s="33">
         <f t="shared" si="0"/>
-        <v>5.5555555555555552E-2</v>
+        <v>7.6388888888888895E-2</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -8730,7 +8765,7 @@
       </c>
       <c r="B10">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C10,'Journal de travail'!$D$7:$D$532)</f>
-        <v>45</v>
+        <v>85</v>
       </c>
       <c r="C10" s="37" t="str">
         <f>'Journal de travail'!M14</f>
@@ -8738,7 +8773,7 @@
       </c>
       <c r="D10" s="33">
         <f t="shared" si="0"/>
-        <v>3.125E-2</v>
+        <v>5.9027777777777776E-2</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -8765,7 +8800,7 @@
       </c>
       <c r="D12" s="34">
         <f>SUM(D4:D11)</f>
-        <v>9.375E-2</v>
+        <v>0.18750000000000003</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -9002,15 +9037,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
@@ -9019,6 +9045,15 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9041,14 +9076,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -9057,4 +9084,12 @@
     <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add: ajout de la page de recherche
[45][WIP]
</commit_message>
<xml_diff>
--- a/Journal de travail/Journal-de-Travail_NomPrénom.xlsx
+++ b/Journal de travail/Journal-de-Travail_NomPrénom.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pt52png\Documents\GitHub\P_mobile\Journal de travail\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00C54833-B6AB-42D6-9266-D742F538BA22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E543567-68A5-423B-87B6-6E9E2BFFDA81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="41">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -152,6 +152,18 @@
   </si>
   <si>
     <t>page de livre + navigation</t>
+  </si>
+  <si>
+    <t>Explication de Monsieur Benfares sur les transformers(AI)</t>
+  </si>
+  <si>
+    <t>Documentation sur comment connecter le backend a l'application MAUI</t>
+  </si>
+  <si>
+    <t>https://learn.microsoft.com/en-us/dotnet/maui/data-cloud/rest?view=net-maui-9.0 | https://learn.microsoft.com/en-us/dotnet/maui/data-cloud/local-web-services?view=net-maui-8.0</t>
+  </si>
+  <si>
+    <t>page de Recherche WIP</t>
   </si>
 </sst>
 </file>
@@ -1086,16 +1098,16 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.6805555555555552E-2</c:v>
+                  <c:v>0.11805555555555555</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.4722222222222224E-2</c:v>
+                  <c:v>6.5972222222222224E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9.0277777777777776E-2</c:v>
+                  <c:v>0.12152777777777778</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -2017,7 +2029,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F17" sqref="F17"/>
+      <selection pane="bottomLeft" activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2070,7 +2082,7 @@
       </c>
       <c r="C3" s="22" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 6 heurs 40 minutes</v>
+        <v>0 jours 8 heurs 55 minutes</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="3"/>
@@ -2089,11 +2101,11 @@
       </c>
       <c r="D4" s="22">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>220</v>
+        <v>355</v>
       </c>
       <c r="E4" s="40">
         <f>SUM(C4:D4)</f>
-        <v>400</v>
+        <v>535</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2399,45 +2411,71 @@
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="16" t="str">
+      <c r="A17" s="16">
         <f>IF(ISBLANK(B17),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B17))</f>
-        <v/>
-      </c>
-      <c r="B17" s="46"/>
+        <v>15</v>
+      </c>
+      <c r="B17" s="46">
+        <v>45758</v>
+      </c>
       <c r="C17" s="47"/>
-      <c r="D17" s="48"/>
-      <c r="E17" s="49"/>
-      <c r="F17" s="36"/>
+      <c r="D17" s="48">
+        <v>45</v>
+      </c>
+      <c r="E17" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="F17" s="36" t="s">
+        <v>37</v>
+      </c>
       <c r="G17" s="52"/>
       <c r="O17">
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="str">
+    <row r="18" spans="1:15" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A18" s="8">
         <f>IF(ISBLANK(B18),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B18))</f>
-        <v/>
-      </c>
-      <c r="B18" s="42"/>
+        <v>15</v>
+      </c>
+      <c r="B18" s="42">
+        <v>45758</v>
+      </c>
       <c r="C18" s="43"/>
-      <c r="D18" s="44"/>
-      <c r="E18" s="45"/>
-      <c r="F18" s="36"/>
-      <c r="G18" s="51"/>
+      <c r="D18" s="44">
+        <v>45</v>
+      </c>
+      <c r="E18" s="45" t="s">
+        <v>6</v>
+      </c>
+      <c r="F18" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="G18" s="51" t="s">
+        <v>39</v>
+      </c>
       <c r="O18">
         <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="16" t="str">
+      <c r="A19" s="16">
         <f>IF(ISBLANK(B19),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B19))</f>
-        <v/>
-      </c>
-      <c r="B19" s="46"/>
+        <v>15</v>
+      </c>
+      <c r="B19" s="46">
+        <v>45758</v>
+      </c>
       <c r="C19" s="47"/>
-      <c r="D19" s="48"/>
-      <c r="E19" s="49"/>
-      <c r="F19" s="36"/>
+      <c r="D19" s="48">
+        <v>45</v>
+      </c>
+      <c r="E19" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="F19" s="36" t="s">
+        <v>40</v>
+      </c>
       <c r="G19" s="52"/>
       <c r="O19">
         <v>55</v>
@@ -8705,7 +8743,7 @@
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="C5" s="41" t="str">
         <f>'Journal de travail'!M9</f>
@@ -8713,7 +8751,7 @@
       </c>
       <c r="D5" s="33">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>8.6805555555555552E-2</v>
+        <v>0.11805555555555555</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -8741,7 +8779,7 @@
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>50</v>
+        <v>95</v>
       </c>
       <c r="C7" s="27" t="str">
         <f>'Journal de travail'!M11</f>
@@ -8749,7 +8787,7 @@
       </c>
       <c r="D7" s="33">
         <f t="shared" si="0"/>
-        <v>3.4722222222222224E-2</v>
+        <v>6.5972222222222224E-2</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -8759,7 +8797,7 @@
       </c>
       <c r="B8">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C8,'Journal de travail'!$D$7:$D$532)</f>
-        <v>70</v>
+        <v>115</v>
       </c>
       <c r="C8" s="28" t="str">
         <f>'Journal de travail'!M12</f>
@@ -8767,7 +8805,7 @@
       </c>
       <c r="D8" s="33">
         <f t="shared" si="0"/>
-        <v>9.0277777777777776E-2</v>
+        <v>0.12152777777777778</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -8830,7 +8868,7 @@
       </c>
       <c r="D12" s="34">
         <f>SUM(D4:D11)</f>
-        <v>0.27777777777777773</v>
+        <v>0.37152777777777779</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>